<commit_message>
3.0.11 Implement strictNullable option. Default false. on true, depend " | undefined | null" to type of nullable properties.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgSourceFileValueObject.xlsx
+++ b/meta/program/BlancoCgSourceFileValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BCF1306-CC3E-E54D-AC0D-6A3783111F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECCE07-FB1B-D949-AC06-0224D709057D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="700" windowWidth="20760" windowHeight="15220" tabRatio="640"/>
+    <workbookView xWindow="10360" yWindow="700" windowWidth="20760" windowHeight="15220" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -387,6 +387,20 @@
     </rPh>
     <rPh sb="28" eb="29">
       <t xml:space="preserve">アタイ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>isStrictNullable</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>nullableな型に対して | undefined | null を追加付与するかどうかのフラグです</t>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">カタ </t>
+    </rPh>
+    <rPh sb="35" eb="39">
+      <t xml:space="preserve">ツイカフヨ </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -394,7 +408,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -777,16 +791,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -889,20 +902,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,7 +932,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1332,14 +1344,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1355,7 +1367,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1378,47 +1390,47 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="D9"/>
@@ -1426,21 +1438,21 @@
       <c r="F9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="36"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D11"/>
@@ -1448,11 +1460,11 @@
       <c r="F11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="37" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D12"/>
@@ -1460,21 +1472,21 @@
       <c r="F12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="36"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
@@ -1486,354 +1498,373 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="52"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="45"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="52"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="41"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="40"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="26"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="42"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="41"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="30"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" ht="56.25" customHeight="1">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="51" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="52"/>
+      <c r="F27" s="50"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <f>A27+1</f>
         <v>2</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24" t="s">
+      <c r="D28" s="22"/>
+      <c r="E28" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="25"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="21">
-        <f t="shared" ref="A29:A40" si="0">A28+1</f>
+      <c r="A29" s="20">
+        <f t="shared" ref="A29:A41" si="0">A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="25"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="21">
+      <c r="A31" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24" t="s">
+      <c r="D31" s="22"/>
+      <c r="E31" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="25"/>
+      <c r="F31" s="24"/>
     </row>
     <row r="32" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A32" s="21">
+      <c r="A32" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <v>4</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A33" s="21">
+      <c r="A33" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="53" t="s">
+      <c r="E33" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="48"/>
     </row>
     <row r="34" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A34" s="21">
+      <c r="A34" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="55"/>
+      <c r="F34" s="53"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="21">
+      <c r="A35" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="44"/>
+      <c r="F35" s="42"/>
     </row>
     <row r="36" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A36" s="21">
+      <c r="A36" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="48"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="21">
+      <c r="A37" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="25"/>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="21">
+      <c r="A38" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="25"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="24"/>
     </row>
     <row r="39" spans="1:6" ht="114.75" customHeight="1">
-      <c r="A39" s="21">
+      <c r="A39" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="49" t="s">
+      <c r="D39" s="22"/>
+      <c r="E39" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="50"/>
+      <c r="F39" s="48"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="21">
+      <c r="A40" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="28" t="b">
+      <c r="D40" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="29"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1856,23 +1887,23 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1885,7 +1916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1913,54 +1944,54 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="33"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="38"/>
-      <c r="D4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="40"/>
+      <c r="B6" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>